<commit_message>
First set of changes to match file template
</commit_message>
<xml_diff>
--- a/sample/input/reg10.xlsx
+++ b/sample/input/reg10.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paisible\Desktop\492\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\casto\git\grams\ipxact-register-generator\sample\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5AE118-1DDA-4CFF-A406-057B9895C9A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="36">
   <si>
     <t xml:space="preserve"> Register List</t>
   </si>
@@ -134,7 +133,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -446,7 +445,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -462,7 +461,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -537,6 +536,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -572,6 +588,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -747,14 +780,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53:B56"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -882,7 +915,9 @@
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
+      <c r="E7" s="27" t="s">
+        <v>9</v>
+      </c>
       <c r="F7" s="14" t="s">
         <v>13</v>
       </c>
@@ -904,9 +939,7 @@
       <c r="D8" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>9</v>
-      </c>
+      <c r="E8" s="15"/>
       <c r="F8" s="17" t="s">
         <v>14</v>
       </c>
@@ -927,9 +960,7 @@
       <c r="D9" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E9" s="15"/>
       <c r="F9" s="17" t="s">
         <v>14</v>
       </c>
@@ -950,9 +981,7 @@
       <c r="D10" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E10" s="15"/>
       <c r="F10" s="17" t="s">
         <v>14</v>
       </c>
@@ -974,9 +1003,7 @@
       <c r="D11" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E11" s="15"/>
       <c r="F11" s="17" t="s">
         <v>14</v>
       </c>
@@ -996,7 +1023,9 @@
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="30"/>
-      <c r="E12" s="27"/>
+      <c r="E12" s="27" t="s">
+        <v>11</v>
+      </c>
       <c r="F12" s="14" t="s">
         <v>13</v>
       </c>
@@ -1018,9 +1047,7 @@
       <c r="D13" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E13" s="15"/>
       <c r="F13" s="17" t="s">
         <v>14</v>
       </c>
@@ -1042,9 +1069,7 @@
       <c r="D14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E14" s="15"/>
       <c r="F14" s="17" t="s">
         <v>14</v>
       </c>
@@ -1067,9 +1092,7 @@
       <c r="D15" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E15" s="15"/>
       <c r="F15" s="17" t="s">
         <v>14</v>
       </c>
@@ -1092,9 +1115,7 @@
       <c r="D16" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E16" s="15"/>
       <c r="F16" s="17" t="s">
         <v>14</v>
       </c>
@@ -1114,7 +1135,9 @@
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="30"/>
-      <c r="E17" s="27"/>
+      <c r="E17" s="27" t="s">
+        <v>11</v>
+      </c>
       <c r="F17" s="14" t="s">
         <v>13</v>
       </c>
@@ -1137,9 +1160,7 @@
       <c r="D18" s="29">
         <v>0</v>
       </c>
-      <c r="E18" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E18" s="15"/>
       <c r="F18" s="17" t="s">
         <v>14</v>
       </c>
@@ -1162,9 +1183,7 @@
       <c r="D19" s="29">
         <v>0</v>
       </c>
-      <c r="E19" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E19" s="15"/>
       <c r="F19" s="17" t="s">
         <v>14</v>
       </c>
@@ -1187,9 +1206,7 @@
       <c r="D20" s="29">
         <v>2</v>
       </c>
-      <c r="E20" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E20" s="15"/>
       <c r="F20" s="17" t="s">
         <v>14</v>
       </c>
@@ -1211,9 +1228,7 @@
       <c r="D21" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E21" s="15"/>
       <c r="F21" s="17" t="s">
         <v>14</v>
       </c>
@@ -1233,7 +1248,9 @@
       </c>
       <c r="C22" s="27"/>
       <c r="D22" s="26"/>
-      <c r="E22" s="27"/>
+      <c r="E22" s="27" t="s">
+        <v>9</v>
+      </c>
       <c r="F22" s="14" t="s">
         <v>13</v>
       </c>
@@ -1255,9 +1272,7 @@
       <c r="D23" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="15" t="s">
-        <v>9</v>
-      </c>
+      <c r="E23" s="15"/>
       <c r="F23" s="17" t="s">
         <v>14</v>
       </c>
@@ -1278,9 +1293,7 @@
       <c r="D24" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E24" s="15"/>
       <c r="F24" s="17" t="s">
         <v>14</v>
       </c>
@@ -1301,9 +1314,7 @@
       <c r="D25" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E25" s="15"/>
       <c r="F25" s="17" t="s">
         <v>14</v>
       </c>
@@ -1325,9 +1336,7 @@
       <c r="D26" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E26" s="15"/>
       <c r="F26" s="17" t="s">
         <v>14</v>
       </c>
@@ -1347,7 +1356,9 @@
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="30"/>
-      <c r="E27" s="27"/>
+      <c r="E27" s="27" t="s">
+        <v>11</v>
+      </c>
       <c r="F27" s="14" t="s">
         <v>13</v>
       </c>
@@ -1369,9 +1380,7 @@
       <c r="D28" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E28" s="15"/>
       <c r="F28" s="17" t="s">
         <v>14</v>
       </c>
@@ -1393,9 +1402,7 @@
       <c r="D29" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E29" s="15"/>
       <c r="F29" s="17" t="s">
         <v>14</v>
       </c>
@@ -1417,9 +1424,7 @@
       <c r="D30" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E30" s="15"/>
       <c r="F30" s="17" t="s">
         <v>14</v>
       </c>
@@ -1441,9 +1446,7 @@
       <c r="D31" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E31" s="15"/>
       <c r="F31" s="17" t="s">
         <v>14</v>
       </c>
@@ -1462,7 +1465,9 @@
       </c>
       <c r="C32" s="27"/>
       <c r="D32" s="30"/>
-      <c r="E32" s="27"/>
+      <c r="E32" s="27" t="s">
+        <v>11</v>
+      </c>
       <c r="F32" s="14" t="s">
         <v>13</v>
       </c>
@@ -1479,9 +1484,7 @@
       <c r="D33" s="29">
         <v>0</v>
       </c>
-      <c r="E33" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E33" s="15"/>
       <c r="F33" s="17" t="s">
         <v>14</v>
       </c>
@@ -1498,9 +1501,7 @@
       <c r="D34" s="29">
         <v>0</v>
       </c>
-      <c r="E34" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E34" s="15"/>
       <c r="F34" s="17" t="s">
         <v>14</v>
       </c>
@@ -1517,9 +1518,7 @@
       <c r="D35" s="29">
         <v>2</v>
       </c>
-      <c r="E35" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E35" s="15"/>
       <c r="F35" s="17" t="s">
         <v>14</v>
       </c>
@@ -1536,9 +1535,7 @@
       <c r="D36" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E36" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E36" s="15"/>
       <c r="F36" s="17" t="s">
         <v>14</v>
       </c>
@@ -1553,7 +1550,9 @@
       </c>
       <c r="C37" s="27"/>
       <c r="D37" s="26"/>
-      <c r="E37" s="27"/>
+      <c r="E37" s="27" t="s">
+        <v>9</v>
+      </c>
       <c r="F37" s="14" t="s">
         <v>13</v>
       </c>
@@ -1570,9 +1569,7 @@
       <c r="D38" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="15" t="s">
-        <v>9</v>
-      </c>
+      <c r="E38" s="15"/>
       <c r="F38" s="17" t="s">
         <v>14</v>
       </c>
@@ -1588,9 +1585,7 @@
       <c r="D39" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E39" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E39" s="15"/>
       <c r="F39" s="17" t="s">
         <v>14</v>
       </c>
@@ -1606,9 +1601,7 @@
       <c r="D40" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E40" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E40" s="15"/>
       <c r="F40" s="17" t="s">
         <v>14</v>
       </c>
@@ -1625,9 +1618,7 @@
       <c r="D41" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E41" s="15"/>
       <c r="F41" s="17" t="s">
         <v>14</v>
       </c>
@@ -1642,7 +1633,9 @@
       </c>
       <c r="C42" s="27"/>
       <c r="D42" s="30"/>
-      <c r="E42" s="27"/>
+      <c r="E42" s="27" t="s">
+        <v>11</v>
+      </c>
       <c r="F42" s="14" t="s">
         <v>13</v>
       </c>
@@ -1659,9 +1652,7 @@
       <c r="D43" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E43" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E43" s="15"/>
       <c r="F43" s="17" t="s">
         <v>14</v>
       </c>
@@ -1678,9 +1669,7 @@
       <c r="D44" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E44" s="15"/>
       <c r="F44" s="17" t="s">
         <v>14</v>
       </c>
@@ -1697,9 +1686,7 @@
       <c r="D45" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E45" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E45" s="15"/>
       <c r="F45" s="17" t="s">
         <v>14</v>
       </c>
@@ -1716,9 +1703,7 @@
       <c r="D46" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E46" s="15"/>
       <c r="F46" s="17" t="s">
         <v>14</v>
       </c>
@@ -1732,7 +1717,9 @@
       </c>
       <c r="C47" s="27"/>
       <c r="D47" s="30"/>
-      <c r="E47" s="27"/>
+      <c r="E47" s="27" t="s">
+        <v>11</v>
+      </c>
       <c r="F47" s="14" t="s">
         <v>13</v>
       </c>
@@ -1749,9 +1736,7 @@
       <c r="D48" s="29">
         <v>0</v>
       </c>
-      <c r="E48" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E48" s="15"/>
       <c r="F48" s="17" t="s">
         <v>14</v>
       </c>
@@ -1768,9 +1753,7 @@
       <c r="D49" s="29">
         <v>0</v>
       </c>
-      <c r="E49" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E49" s="15"/>
       <c r="F49" s="17" t="s">
         <v>14</v>
       </c>
@@ -1787,9 +1770,7 @@
       <c r="D50" s="29">
         <v>2</v>
       </c>
-      <c r="E50" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E50" s="15"/>
       <c r="F50" s="17" t="s">
         <v>14</v>
       </c>
@@ -1806,9 +1787,7 @@
       <c r="D51" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E51" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E51" s="15"/>
       <c r="F51" s="17" t="s">
         <v>14</v>
       </c>
@@ -1823,7 +1802,9 @@
       </c>
       <c r="C52" s="27"/>
       <c r="D52" s="26"/>
-      <c r="E52" s="27"/>
+      <c r="E52" s="27" t="s">
+        <v>9</v>
+      </c>
       <c r="F52" s="14" t="s">
         <v>13</v>
       </c>
@@ -1840,9 +1821,7 @@
       <c r="D53" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E53" s="15" t="s">
-        <v>9</v>
-      </c>
+      <c r="E53" s="15"/>
       <c r="F53" s="17" t="s">
         <v>14</v>
       </c>
@@ -1858,9 +1837,7 @@
       <c r="D54" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E54" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E54" s="15"/>
       <c r="F54" s="17" t="s">
         <v>14</v>
       </c>
@@ -1876,9 +1853,7 @@
       <c r="D55" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E55" s="15"/>
       <c r="F55" s="17" t="s">
         <v>14</v>
       </c>
@@ -1895,9 +1870,7 @@
       <c r="D56" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E56" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="E56" s="15"/>
       <c r="F56" s="17" t="s">
         <v>14</v>
       </c>
@@ -2161,28 +2134,4 @@
     <ignoredError sqref="D21" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>